<commit_message>
Added data + Analysis files
Data for Flask A, B, E, F. Analysis files on Rmd. Some edited versions of STL files.
</commit_message>
<xml_diff>
--- a/sampler cost.xlsx
+++ b/sampler cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmah/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmah/Documents/GitHub/Automatic water sampler/Automatic-Water-Sampler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4687D64-991E-124D-8B4C-43691BE61A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9617BA0B-6969-5445-AB18-FFCEFE7C93BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{F00E827C-72D0-C24E-A194-146314DC2ED8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{F00E827C-72D0-C24E-A194-146314DC2ED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Auto-sampler" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="72">
   <si>
     <t>Item</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/32816676299.html?spm=a2g0s.9042311.0.0.6f234c4dwMYy9f</t>
+  </si>
+  <si>
+    <t>Plywood Board Base</t>
   </si>
 </sst>
 </file>
@@ -689,11 +692,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C31BE1-8D56-2141-AFA5-90A16ED6BE30}">
   <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="33.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
@@ -1137,7 +1143,7 @@
         <v>1</v>
       </c>
       <c r="E26">
-        <f t="shared" ref="E26:E40" si="0">B26*C26+D26</f>
+        <f t="shared" ref="E26:E41" si="0">B26*C26+D26</f>
         <v>38</v>
       </c>
       <c r="H26" t="s">
@@ -1487,11 +1493,20 @@
     </row>
     <row r="41" spans="1:21">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>71</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
       </c>
       <c r="E41">
-        <f>SUM(E26:E40)</f>
-        <v>146.21</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H41" t="s">
+        <v>26</v>
       </c>
       <c r="P41" s="7"/>
       <c r="Q41" s="2"/>
@@ -1501,6 +1516,13 @@
       <c r="U41" s="2"/>
     </row>
     <row r="42" spans="1:21">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42">
+        <f>SUM(E26:E41)</f>
+        <v>149.21</v>
+      </c>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="4"/>
@@ -1521,8 +1543,8 @@
         <v>62</v>
       </c>
       <c r="E44" s="13">
-        <f>SUM(E9,E16,E23,E41)</f>
-        <v>355.68</v>
+        <f>SUM(E9,E16,E23,E42)</f>
+        <v>358.68</v>
       </c>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
@@ -1588,7 +1610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB31F30-B3B7-7444-8F25-A0911876EECE}">
   <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>

</xml_diff>